<commit_message>
verouillage cellule Create FT
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT LoS.xlsx
+++ b/lib/PHPExcel/templates/FT LoS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -740,12 +740,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -764,9 +760,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -790,99 +783,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -901,9 +828,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -913,29 +837,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -950,70 +856,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
@@ -1023,100 +880,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="centerContinuous"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1131,18 +900,132 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1674,990 +1557,990 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10" style="12" customWidth="1"/>
-    <col min="3" max="3" width="2.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="7" style="12" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="9" style="12" customWidth="1"/>
-    <col min="7" max="7" width="1.28515625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="12" customWidth="1"/>
-    <col min="9" max="10" width="10.140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="8.7109375" style="12"/>
+    <col min="1" max="1" width="14.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10" style="10" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="7" style="10" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9" style="10" customWidth="1"/>
+    <col min="7" max="7" width="1.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="10" customWidth="1"/>
+    <col min="9" max="10" width="10.140625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G1" s="13"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="78" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="139"/>
-      <c r="H5" s="137" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="H5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-      <c r="K5" s="139"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="73"/>
     </row>
     <row r="6" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
-      <c r="H7" s="20" t="s">
+      <c r="B7" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="80"/>
+      <c r="H7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="89"/>
-      <c r="K7" s="95"/>
+      <c r="I7" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="94"/>
-      <c r="H8" s="20" t="s">
+      <c r="B8" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="82"/>
+      <c r="H8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="96"/>
-      <c r="K8" s="97"/>
+      <c r="I8" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="61"/>
+      <c r="K8" s="62"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="94"/>
-      <c r="H9" s="20" t="s">
+      <c r="B9" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="82"/>
+      <c r="H9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="96"/>
-      <c r="K9" s="97"/>
+      <c r="I9" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="61"/>
+      <c r="K9" s="62"/>
     </row>
     <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="H10" s="20" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="H10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="24" t="s">
+      <c r="I10" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="95"/>
+      <c r="K10" s="60"/>
     </row>
     <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="89"/>
-      <c r="K11" s="95"/>
+      <c r="I11" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="59"/>
+      <c r="K11" s="60"/>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="25"/>
-      <c r="H12" s="20" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="23"/>
+      <c r="H12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" s="96"/>
-      <c r="K12" s="97"/>
+      <c r="I12" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="61"/>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27" t="s">
+      <c r="B13" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="83"/>
+      <c r="D13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28" t="s">
+      <c r="E13" s="24"/>
+      <c r="F13" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="82"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="86"/>
     </row>
     <row r="14" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="32"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="41"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="21"/>
     </row>
     <row r="15" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27" t="s">
+      <c r="B15" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="83"/>
+      <c r="D15" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="N15" s="27"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="N15" s="24"/>
     </row>
     <row r="16" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27" t="s">
+      <c r="B16" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="83"/>
+      <c r="D16" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="H16" s="137" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="138"/>
-      <c r="J16" s="138"/>
-      <c r="K16" s="139"/>
-      <c r="N16" s="27"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="K16" s="73"/>
+      <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="27" t="s">
+      <c r="B17" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="20" t="s">
+      <c r="E17" s="24"/>
+      <c r="F17" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="K17" s="99"/>
-      <c r="N17" s="27"/>
+      <c r="J17" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" s="60"/>
+      <c r="N17" s="24"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="102"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="27" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="62"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="K18" s="101"/>
+      <c r="J18" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="62"/>
     </row>
     <row r="19" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="40"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="21"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="90"/>
     </row>
     <row r="20" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="I20" s="112"/>
-      <c r="J20" s="41" t="s">
+      <c r="I20" s="91"/>
+      <c r="J20" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="113" t="s">
+      <c r="K20" s="92" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="137" t="s">
+      <c r="A21" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="139"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="84" t="s">
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="73"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="135"/>
+      <c r="K21" s="94"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="43"/>
-      <c r="H22" s="20" t="s">
+      <c r="A22" s="15"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="H22" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="134" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" s="42" t="s">
+      <c r="I22" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="133" t="s">
+      <c r="K22" s="96" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="89" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="44" t="s">
+      <c r="B23" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="45" t="s">
+      <c r="F23" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" s="42" t="s">
+      <c r="I23" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="114" t="s">
+      <c r="K23" s="98" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="44" t="s">
+      <c r="B24" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="130" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" s="9" t="s">
+      <c r="I24" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="129" t="s">
+      <c r="K24" s="100" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="92" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="44" t="s">
+      <c r="B25" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="130" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="I25" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="8"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="47"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="2" t="s">
+      <c r="A26" s="18"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="34"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="46" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46" t="s">
+      <c r="C27" s="33"/>
+      <c r="D27" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="48"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="3" t="s">
+      <c r="E27" s="33"/>
+      <c r="F27" s="34"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="6"/>
+      <c r="K27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="112" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="115"/>
-      <c r="D28" s="116" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="112"/>
-      <c r="F28" s="48"/>
-      <c r="H28" s="7" t="s">
+      <c r="B28" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="101"/>
+      <c r="D28" s="102" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="91"/>
+      <c r="F28" s="34"/>
+      <c r="H28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="120" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="121" t="s">
-        <v>90</v>
-      </c>
-      <c r="K28" s="10"/>
-      <c r="M28" s="136" t="s">
+      <c r="I28" s="103" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="K28" s="105"/>
+      <c r="M28" s="70" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="126" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="127"/>
-      <c r="D29" s="128" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="126"/>
-      <c r="F29" s="48"/>
-      <c r="H29" s="7" t="s">
+      <c r="B29" s="106" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="107"/>
+      <c r="D29" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="106"/>
+      <c r="F29" s="34"/>
+      <c r="H29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="123" t="s">
-        <v>90</v>
-      </c>
-      <c r="K29" s="10"/>
-      <c r="M29" s="136" t="s">
+      <c r="I29" s="109" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="105"/>
+      <c r="M29" s="70" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="117" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="118"/>
-      <c r="D30" s="119" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="117"/>
-      <c r="F30" s="48"/>
-      <c r="H30" s="7" t="s">
+      <c r="B30" s="111" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="112"/>
+      <c r="D30" s="113" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="111"/>
+      <c r="F30" s="34"/>
+      <c r="H30" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="123" t="s">
-        <v>90</v>
-      </c>
-      <c r="K30" s="10"/>
-      <c r="M30" s="136" t="s">
+      <c r="I30" s="109" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" s="105"/>
+      <c r="M30" s="70" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="48"/>
-      <c r="H31" s="7" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="34"/>
+      <c r="H31" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="124" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="125" t="s">
-        <v>90</v>
-      </c>
-      <c r="K31" s="10"/>
+      <c r="I31" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="115" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" s="105"/>
     </row>
     <row r="32" spans="1:14" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="23"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="50"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="21"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="116"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="117"/>
     </row>
     <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="51"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="118"/>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="142" t="s">
+      <c r="A34" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="143"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="85" t="s">
+      <c r="B34" s="119"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="42" t="s">
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="J34" s="106"/>
-      <c r="K34" s="53"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="37"/>
     </row>
     <row r="35" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="54"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="57"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="58"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="99"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="44" t="s">
+      <c r="B36" s="60"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="24" t="s">
+      <c r="E36" s="27"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="J36" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="88" t="s">
+      <c r="K36" s="58" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="92"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="44" t="s">
+      <c r="B37" s="61"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="98"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="42" t="s">
+      <c r="E37" s="27"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="I37" s="89"/>
-      <c r="J37" s="89"/>
-      <c r="K37" s="95"/>
-      <c r="M37" s="44"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="44"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="60"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="59" t="s">
+      <c r="A38" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="23"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="44"/>
-      <c r="O38" s="44"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="21"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
     </row>
     <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
-      <c r="O39" s="44"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
     </row>
     <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="137" t="s">
+      <c r="A40" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="138"/>
-      <c r="C40" s="138"/>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138"/>
-      <c r="J40" s="138"/>
-      <c r="K40" s="139"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="44"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="73"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
     </row>
     <row r="41" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="75"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="62" t="s">
+      <c r="A41" s="51"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="121"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="I41" s="63" t="s">
+      <c r="I41" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="J41" s="18"/>
-      <c r="K41" s="64"/>
-      <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
-      <c r="O41" s="44"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="41"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
     </row>
     <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="65" t="s">
+      <c r="B42" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="66" t="s">
+      <c r="C42" s="20"/>
+      <c r="D42" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="E42" s="67"/>
-      <c r="F42" s="65" t="s">
+      <c r="E42" s="44"/>
+      <c r="F42" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="G42" s="22"/>
-      <c r="H42" s="66" t="s">
+      <c r="G42" s="20"/>
+      <c r="H42" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="I42" s="65" t="s">
+      <c r="I42" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="J42" s="66" t="s">
+      <c r="J42" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="68" t="s">
+      <c r="K42" s="45" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N43" s="69"/>
-      <c r="O43" s="39"/>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="39"/>
-      <c r="R43" s="39"/>
-      <c r="S43" s="44"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="89"/>
+      <c r="P43" s="89"/>
+      <c r="Q43" s="89"/>
+      <c r="R43" s="89"/>
+      <c r="S43" s="32"/>
     </row>
     <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="137" t="s">
+      <c r="A44" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="138"/>
-      <c r="C44" s="138"/>
-      <c r="D44" s="138"/>
-      <c r="E44" s="138"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="138"/>
-      <c r="H44" s="138"/>
-      <c r="I44" s="139"/>
-      <c r="J44" s="144" t="s">
+      <c r="B44" s="72"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="K44" s="145"/>
+      <c r="K44" s="77"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="107"/>
-      <c r="C45" s="44"/>
-      <c r="E45" s="42" t="s">
+      <c r="B45" s="64"/>
+      <c r="C45" s="32"/>
+      <c r="E45" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="70"/>
-      <c r="G45" s="44" t="s">
+      <c r="F45" s="122"/>
+      <c r="G45" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="H45" s="44"/>
-      <c r="I45" s="110"/>
-      <c r="J45" s="72" t="s">
+      <c r="H45" s="32"/>
+      <c r="I45" s="66"/>
+      <c r="J45" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="K45" s="73"/>
+      <c r="K45" s="49"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44" t="s">
+      <c r="A46" s="18"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="132" t="s">
-        <v>90</v>
-      </c>
-      <c r="K46" s="105"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="K46" s="123"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="98"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44" t="s">
+      <c r="B47" s="59"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="H47" s="44"/>
-      <c r="I47" s="99"/>
-      <c r="J47" s="71" t="s">
+      <c r="H47" s="32"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="K47" s="48"/>
+      <c r="K47" s="34"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="73"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="49"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="77"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="78" t="s">
+      <c r="B49" s="52"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="77"/>
-      <c r="H49" s="111"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="131" t="s">
-        <v>90</v>
-      </c>
-      <c r="K49" s="104"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="K49" s="63"/>
     </row>
     <row r="50" spans="1:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="140"/>
-      <c r="K50" s="141"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="124"/>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="74" t="s">
+      <c r="A52" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="11" t="s">
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I52" s="108" t="s">
-        <v>90</v>
-      </c>
-      <c r="J52" s="11" t="s">
+      <c r="I52" s="125" t="s">
+        <v>90</v>
+      </c>
+      <c r="J52" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="K52" s="109" t="s">
+      <c r="K52" s="65" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
-      <c r="B53" s="44"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="48"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="34"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="48"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="34"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="20"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="48"/>
+      <c r="A55" s="18"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="34"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="48"/>
+      <c r="A56" s="18"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="34"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="48"/>
+      <c r="A57" s="18"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="34"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="20"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="44"/>
-      <c r="I58" s="44"/>
-      <c r="J58" s="44"/>
-      <c r="K58" s="48"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="34"/>
     </row>
     <row r="59" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="44"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="32"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="136" t="s">
+      <c r="A60" s="70" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FT : ajout commentaire + fix extenso LoS/Dwl
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT LoS.xlsx
+++ b/lib/PHPExcel/templates/FT LoS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -740,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1027,6 +1027,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2448,7 +2449,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="18"/>
+      <c r="A53" s="126"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
       <c r="D53" s="32"/>

</xml_diff>